<commit_message>
updated bcrbq, becf, mpcbs, bfpat
</commit_message>
<xml_diff>
--- a/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
+++ b/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamho\Dropbox\Energy Innovation\InputData_Working\홍상현\elec\MPCbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SD_Card\Dropbox\재현\EPS\InputData_Complete\elec\MPCbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43ED7B38-CF4E-4F87-944D-3589E565A034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA40B315-DD85-499C-B68C-3F026FD16861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="1290" windowWidth="28830" windowHeight="18770" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>We used the market potential of renewable energy sources</t>
+    <t>We used the technical potential of renewable energy sources</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -537,21 +537,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="60.83203125" customWidth="1"/>
+    <col min="2" max="2" width="60.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,37 +559,37 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B5" s="3">
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -609,19 +609,19 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.4140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="71" customWidth="1"/>
-    <col min="5" max="5" width="16.25" customWidth="1"/>
+    <col min="5" max="5" width="16.19921875" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -629,7 +629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -638,7 +638,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -647,7 +647,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -656,31 +656,31 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
-        <v>24000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+        <v>352000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>369000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+        <v>2409000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -690,24 +690,23 @@
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9">
-        <f>Data!B21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>334000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+        <v>1259000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -716,7 +715,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -725,7 +724,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -734,15 +733,15 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14">
-        <v>41000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+        <v>387000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -751,7 +750,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -760,7 +759,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -782,17 +781,17 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="27.25" customWidth="1"/>
+    <col min="2" max="2" width="27.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -800,7 +799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -809,7 +808,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -818,7 +817,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -827,34 +826,34 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="6">
         <f>Data!B5</f>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="6">
         <f>Data!B6</f>
-        <v>24000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>352000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="6">
         <f>Data!B7</f>
-        <v>369000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2409000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -863,25 +862,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="6">
         <f>Data!B9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="6">
         <f>Data!B10</f>
-        <v>334000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1259000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -890,7 +889,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -899,7 +898,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -908,16 +907,16 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="6">
         <f>Data!B14</f>
-        <v>41000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+        <v>387000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -926,7 +925,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -935,7 +934,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
electricity fixes for solid waste and geothermal mpcbs and syc
</commit_message>
<xml_diff>
--- a/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
+++ b/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\elec\MPCbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\South Korea\eps-southkorea\InputData\elec\MPCbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F1D675-3657-4A98-8128-9E83AD7463BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4A2C01-11F2-4F76-A706-0CAB1E36B5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12670" yWindow="360" windowWidth="12170" windowHeight="13030" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -537,13 +537,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="60.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -609,15 +609,15 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="71" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -703,7 +703,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>1259000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -763,7 +763,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="6">
-        <v>4000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -780,14 +780,14 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -876,7 +876,7 @@
       </c>
       <c r="B10" s="6">
         <f>Data!B10</f>
-        <v>1259000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -939,7 +939,7 @@
       </c>
       <c r="B17" s="6">
         <f>Data!B17</f>
-        <v>4000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cap petroleum and HFO plants
</commit_message>
<xml_diff>
--- a/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
+++ b/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\South Korea\eps-southkorea\InputData\elec\MPCbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\elec\MPCbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4A2C01-11F2-4F76-A706-0CAB1E36B5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF38B70-C831-4E14-8B28-39677A3B6BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12670" yWindow="360" windowWidth="12170" windowHeight="13030" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Source:</t>
   </si>
@@ -118,6 +118,12 @@
   <si>
     <t>We used the technical potential of renewable energy sources</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>As peaking needs are expected to be met by gas in Korea, we limit petroleum and</t>
+  </si>
+  <si>
+    <t>heavy fuel oil plants at current capacity.</t>
   </si>
 </sst>
 </file>
@@ -535,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -592,6 +598,16 @@
     <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -780,8 +796,8 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -884,8 +900,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="6">
-        <f>Data!B11</f>
-        <v>9000000000000</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -893,7 +908,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="6">
-        <f>B11</f>
+        <f>B3</f>
         <v>9000000000000</v>
       </c>
     </row>
@@ -929,8 +944,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="6">
-        <f>Data!B16</f>
-        <v>9000000000000</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="17" spans="1:2">

</xml_diff>